<commit_message>
feat: update the data file
</commit_message>
<xml_diff>
--- a/evolution/data/variables EVOLUTIONS.xlsx
+++ b/evolution/data/variables EVOLUTIONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FontyColoBe\Documents\GitHub\cereq-dataviz\evolution\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Datavizzz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789B8878-8F1A-46D4-B04F-821399B95A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC02DD09-814F-4206-94AD-F5BD0FF9F8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{0FDA0247-04C8-41EE-A704-5099EBC3E1E6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0FDA0247-04C8-41EE-A704-5099EBC3E1E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -50,39 +50,24 @@
     <t>taux_emploi</t>
   </si>
   <si>
-    <t>Taux d’emploi à trois ans</t>
-  </si>
-  <si>
     <t>part_chomage</t>
   </si>
   <si>
-    <t>Proportion de sortants au chômage à trois ans</t>
-  </si>
-  <si>
     <t>taux_chomage</t>
   </si>
   <si>
-    <t>Taux de chômage à trois ans</t>
-  </si>
-  <si>
     <t>Le taux de chômage correspond à la part des  individus sans emploi et à la recherche d'un emploi parmi les actifs (individus en emploi ou au chômage)</t>
   </si>
   <si>
     <t>taux_edi</t>
   </si>
   <si>
-    <t>Proportion de sortants en emploi à durée indéterminé à trois ans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Proportion d'individus en emploi non-salarié (personne à son compte ou aide familial), en contrat à durée indéterminée (CDI) ou avec le statut de fonctionnaire </t>
   </si>
   <si>
     <t>revenu_travail</t>
   </si>
   <si>
-    <t xml:space="preserve">Revenu mensuel médian à trois ans </t>
-  </si>
-  <si>
     <t>Niveau de salaire ou traitement mensuel net primes incluses médian. Le revenu médian est la valeur telle que la moitié des individus de la population considérée gagne plus, l'autre moitié gagne  moins.</t>
   </si>
   <si>
@@ -92,6 +77,9 @@
     <t>Proportion de sortants cadres à trois ans</t>
   </si>
   <si>
+    <t>pos_prof_inter</t>
+  </si>
+  <si>
     <t>Proportion de sortants professions intermédiaires à trois ans</t>
   </si>
   <si>
@@ -140,9 +128,6 @@
     <t>part_tps_partiel</t>
   </si>
   <si>
-    <t>Proportion de sortants en emploi à temps partiel à trois ans</t>
-  </si>
-  <si>
     <t>Variable affichée</t>
   </si>
   <si>
@@ -152,7 +137,22 @@
     <t>Non</t>
   </si>
   <si>
-    <t>pos_prof_int</t>
+    <t>Proportion de sortants en emploi à durée indéterminé</t>
+  </si>
+  <si>
+    <t>Proportion de sortants en emploi à temps partiel</t>
+  </si>
+  <si>
+    <t>Revenu mensuel médian</t>
+  </si>
+  <si>
+    <t>Taux d’emploi</t>
+  </si>
+  <si>
+    <t>Proportion de sortants au chômage</t>
+  </si>
+  <si>
+    <t>Taux de chômage</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -557,7 +557,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -571,60 +571,60 @@
     </row>
     <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>34</v>
@@ -632,115 +632,115 @@
     </row>
     <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
fix: add s to the title of the last graphic
</commit_message>
<xml_diff>
--- a/evolution/data/variables EVOLUTIONS.xlsx
+++ b/evolution/data/variables EVOLUTIONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Datavizzz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mouna/Desktop/Work/GitHub/cereq-dataviz/evolution/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC02DD09-814F-4206-94AD-F5BD0FF9F8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4441FC77-FE35-CE4D-9F2E-4ECECB842921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0FDA0247-04C8-41EE-A704-5099EBC3E1E6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20140" xr2:uid="{0FDA0247-04C8-41EE-A704-5099EBC3E1E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>revenu_travail</t>
   </si>
   <si>
-    <t>Niveau de salaire ou traitement mensuel net primes incluses médian. Le revenu médian est la valeur telle que la moitié des individus de la population considérée gagne plus, l'autre moitié gagne  moins.</t>
-  </si>
-  <si>
     <t>pos_cadres</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>Taux de chômage</t>
+  </si>
+  <si>
+    <t>Niveau de salaire ou traitement mensuel net primes incluses médian. Le revenu médian est la valeur telle que la moitié des individus de la population considérée gagne plus, l'autre moitié gagne moins.</t>
   </si>
 </sst>
 </file>
@@ -244,7 +244,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -542,22 +542,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCC49D9-688F-41A5-BE55-128E36F0155B}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="1"/>
-    <col min="2" max="2" width="23.1796875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="103.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.81640625" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="23.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="103.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -569,191 +567,191 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="6" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="6" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="6" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
     </row>
   </sheetData>
@@ -763,6 +761,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e8254419-5e3e-4d09-9ab1-694bd035361a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a3559f96-a391-4298-a476-5fa029e2109e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000DCE2AD71575ED409F6CD8D87660A7B5" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="e7a409e0b47e02996c47cd99ab55c69c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a3559f96-a391-4298-a476-5fa029e2109e" xmlns:ns3="e8254419-5e3e-4d09-9ab1-694bd035361a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ec4d4004c5339e4d0b1f4fd079361e4" ns2:_="" ns3:_="">
     <xsd:import namespace="a3559f96-a391-4298-a476-5fa029e2109e"/>
@@ -985,27 +1003,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C982F7B-9F64-4BB5-A7EE-B02A98A3CE38}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e8254419-5e3e-4d09-9ab1-694bd035361a"/>
+    <ds:schemaRef ds:uri="a3559f96-a391-4298-a476-5fa029e2109e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e8254419-5e3e-4d09-9ab1-694bd035361a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a3559f96-a391-4298-a476-5fa029e2109e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED99F3F-669F-4292-BE5F-AA397ACBBD82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DD558F8-9C61-4625-9943-A9AFF41A0CEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1022,23 +1039,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED99F3F-669F-4292-BE5F-AA397ACBBD82}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C982F7B-9F64-4BB5-A7EE-B02A98A3CE38}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e8254419-5e3e-4d09-9ab1-694bd035361a"/>
-    <ds:schemaRef ds:uri="a3559f96-a391-4298-a476-5fa029e2109e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: update the variables evolutions file
</commit_message>
<xml_diff>
--- a/evolution/data/variables EVOLUTIONS.xlsx
+++ b/evolution/data/variables EVOLUTIONS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mouna/Desktop/Work/GitHub/cereq-dataviz/evolution/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4441FC77-FE35-CE4D-9F2E-4ECECB842921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748796B6-48DC-2445-9D24-A5173DAD47CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20140" xr2:uid="{0FDA0247-04C8-41EE-A704-5099EBC3E1E6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Nom_colonne</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>Niveau de salaire ou traitement mensuel net primes incluses médian. Le revenu médian est la valeur telle que la moitié des individus de la population considérée gagne plus, l'autre moitié gagne moins.</t>
+  </si>
+  <si>
+    <t>comptence_ok</t>
+  </si>
+  <si>
+    <t>La proportion de jeunes estimant être employés à leur niveau de compétence</t>
   </si>
 </sst>
 </file>
@@ -741,17 +747,25 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
     </row>
   </sheetData>
@@ -761,6 +775,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="e8254419-5e3e-4d09-9ab1-694bd035361a" xsi:nil="true"/>
@@ -769,15 +792,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1004,20 +1018,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED99F3F-669F-4292-BE5F-AA397ACBBD82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C982F7B-9F64-4BB5-A7EE-B02A98A3CE38}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="e8254419-5e3e-4d09-9ab1-694bd035361a"/>
     <ds:schemaRef ds:uri="a3559f96-a391-4298-a476-5fa029e2109e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED99F3F-669F-4292-BE5F-AA397ACBBD82}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>